<commit_message>
Make default sheet look nice
</commit_message>
<xml_diff>
--- a/autumn/xls/default_constants.xlsx
+++ b/autumn/xls/default_constants.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="default_constants" sheetId="11" r:id="rId1"/>
+    <sheet name="dropdown_lists" sheetId="12" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>tb_rate_late_progression</t>
   </si>
@@ -65,15 +65,9 @@
     <t>description</t>
   </si>
   <si>
-    <t>evidence for value</t>
-  </si>
-  <si>
     <t>tb_multiplier_latency_protection</t>
   </si>
   <si>
-    <t>..\settings\pdf\protection_latency_andrews2012.pdf</t>
-  </si>
-  <si>
     <t>Relative risk of infection in those already latently infected</t>
   </si>
   <si>
@@ -243,16 +237,26 @@
   </si>
   <si>
     <t>scenarios_to_run</t>
+  </si>
+  <si>
+    <t>scipy</t>
+  </si>
+  <si>
+    <t>explicit</t>
+  </si>
+  <si>
+    <t>Don't change this - change through control panel please</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,29 +319,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="3" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="6" tint="-0.249977111117893"/>
+      <color theme="6" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,12 +379,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -385,8 +389,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -444,142 +460,11 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -594,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="665">
+  <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -1259,60 +1144,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="664"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="9" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="665">
+  <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
     <cellStyle name="Comma 2 2" xfId="6"/>
-    <cellStyle name="Hyperlink" xfId="664" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Input 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2274,541 +2160,615 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="52.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="28">
+        <v>15</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B3" s="25">
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7">
+    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="25">
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B7" s="25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="7">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7">
+      <c r="B8" s="25">
         <f>1/15</f>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="25">
+        <v>0.21</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="25">
         <f>60/365.251</f>
         <v>0.16427059747954148</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B14" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B15" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B16" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B17" s="25">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B18" s="25">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B19" s="25">
         <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B20" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B21" s="25">
         <f>6.8/1000000*365</f>
         <v>2.4819999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="8">
+    </row>
+    <row r="23" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="20">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="20">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="20">
         <f>1/52</f>
         <v>1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="26" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="25">
         <v>26</v>
       </c>
-      <c r="B22" s="8">
+      <c r="C26" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="25">
+        <v>4</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="25">
+        <v>2</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="26">
         <v>0.4</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="C29" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="8">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="B30" s="22">
+        <v>4.7</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="8">
-        <v>0.51500000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="8">
-        <v>4.7</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="7">
-        <v>15</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="7">
-        <v>26</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+    </row>
+    <row r="31" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="35">
+        <v>1895</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="35">
+        <v>2016</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="35">
+        <v>2020</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="7">
-        <v>4</v>
-      </c>
-      <c r="C28" s="12" t="s">
+      <c r="B35" s="36">
+        <v>1945</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="36" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="7">
-        <v>1945</v>
-      </c>
-      <c r="C29" s="12" t="s">
+      <c r="B36" s="36">
+        <v>1955</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+    <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="7">
-        <v>1955</v>
-      </c>
-      <c r="C30" s="12" t="s">
+      <c r="B37" s="36">
+        <v>2050</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="7">
-        <v>2050</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="7">
-        <v>2</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="14">
-        <v>0.4</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+    <row r="38" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="35">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="35">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="16">
-        <v>1895</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="B40" s="35">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="16">
-        <v>2016</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="B41" s="35">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="35">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="16">
-        <v>2020</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="B43" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+    <row r="44" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="18">
-        <v>1000000</v>
-      </c>
-      <c r="C37" s="17" t="s">
+      <c r="B44" s="33">
+        <v>3</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+    <row r="45" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B45" s="30">
         <v>3</v>
       </c>
-      <c r="C38" s="17" t="s">
+    </row>
+    <row r="46" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="B46" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="8">
+      <c r="B47" s="31">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="8">
+    <row r="48" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="20">
-        <v>1990</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="22">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="22">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="22">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
+    <row r="49" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="23">
-        <v>2035</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="B52" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="25">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="B53" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
+      <c r="B54" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="29">
+    </row>
+    <row r="55" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:B47 B52">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B44">
+      <formula1>0</formula1>
+      <formula2>10000000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32:B42">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B18:B19 B8 B11 B21" unlockedFormula="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B48:B51</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B54</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B55</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr published="0"/>
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B53" s="35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="39"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="B17:B18 B7 B10 B20" unlockedFormula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>